<commit_message>
10.15 optimization hw2 & modify dm hw1
</commit_message>
<xml_diff>
--- a/MDS2020 Data Mining/hw1/answer book-hw1.xlsx
+++ b/MDS2020 Data Mining/hw1/answer book-hw1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codes\GraduateCourses\MDS2020 Data Mining\hw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E73426-2096-4FE5-A1F7-82FEF6A267BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2072D40F-533F-40C5-B440-A63FA376CA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -614,9 +614,6 @@
     </r>
   </si>
   <si>
-    <t>Leaf nodes: 15</t>
-  </si>
-  <si>
     <t>Refer to https://scikit-learn.org/stable/modules/generated/sklearn.tree.DecisionTreeClassifier.html</t>
   </si>
   <si>
@@ -647,9 +644,6 @@
       </rPr>
       <t xml:space="preserve"> in the tree?</t>
     </r>
-  </si>
-  <si>
-    <t>Total nodes: 29</t>
   </si>
   <si>
     <t>Refer to https://scikit-learn.org/stable/auto_examples/tree/plot_unveil_tree_structure.html</t>
@@ -765,6 +759,14 @@
       </rPr>
       <t xml:space="preserve"> (¥123,606,400.23)</t>
     </r>
+  </si>
+  <si>
+    <t>Leaf nodes: 12</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total nodes: 23</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1249,8 +1251,8 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -1264,12 +1266,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1288,7 +1290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="31" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1296,7 +1298,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="5">
         <v>5</v>
@@ -1305,7 +1307,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="46" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1313,7 +1315,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="5">
         <v>10</v>
@@ -1322,7 +1324,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="31" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1330,7 +1332,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="5">
         <v>10</v>
@@ -1347,7 +1349,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="5">
         <v>5</v>
@@ -1368,7 +1370,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D8" s="5">
         <v>10</v>
@@ -1377,7 +1379,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="61" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -1385,7 +1387,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="5">
         <v>10</v>
@@ -1394,7 +1396,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="62" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1402,7 +1404,7 @@
         <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10" s="5">
         <v>10</v>
@@ -1419,7 +1421,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D11" s="5">
         <v>15</v>
@@ -1453,37 +1455,37 @@
         <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D14" s="5">
         <v>5</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D15" s="5">
         <v>5</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="C16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="9">
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="4">
         <f>SUM(D3:D15)</f>
         <v>100</v>
       </c>

</xml_diff>